<commit_message>
Refactoring: New templates for the new formatter in templates, no longer in Excel
</commit_message>
<xml_diff>
--- a/data/mock_data/mock_data.xlsx
+++ b/data/mock_data/mock_data.xlsx
@@ -7,102 +7,87 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Data" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+  <si>
+    <t>client_id</t>
+  </si>
   <si>
     <t>client_name</t>
   </si>
   <si>
-    <t>string;upper</t>
-  </si>
-  <si>
-    <t>John Doe</t>
-  </si>
-  <si>
-    <t>Jane Smith</t>
-  </si>
-  <si>
-    <t>Acme Corp</t>
+    <t>contract_date</t>
   </si>
   <si>
     <t>contract_value</t>
   </si>
   <si>
-    <t>currency;USD</t>
-  </si>
-  <si>
-    <t>start_date</t>
-  </si>
-  <si>
-    <t>date;long</t>
-  </si>
-  <si>
-    <t>2024-01-15</t>
-  </si>
-  <si>
-    <t>2024-02-01</t>
-  </si>
-  <si>
-    <t>2024-03-10</t>
-  </si>
-  <si>
-    <t>tax_id</t>
-  </si>
-  <si>
-    <t>mask;###-##-####</t>
-  </si>
-  <si>
-    <t>123456789</t>
-  </si>
-  <si>
-    <t>987654321</t>
-  </si>
-  <si>
-    <t>555666777</t>
-  </si>
-  <si>
-    <t>risk_level</t>
-  </si>
-  <si>
-    <t>string;title</t>
-  </si>
-  <si>
-    <t>low</t>
-  </si>
-  <si>
-    <t>high</t>
-  </si>
-  <si>
-    <t>medium</t>
+    <t>completion_rate</t>
+  </si>
+  <si>
+    <t>is_active</t>
+  </si>
+  <si>
+    <t>has_debt</t>
+  </si>
+  <si>
+    <t>status_code</t>
+  </si>
+  <si>
+    <t>client_photo</t>
   </si>
   <si>
     <t>signature_img</t>
   </si>
   <si>
-    <t>image;4;2</t>
-  </si>
-  <si>
-    <t>sig_john.png</t>
-  </si>
-  <si>
-    <t>sig_jane.png</t>
-  </si>
-  <si>
-    <t>sig_corp.png</t>
+    <t>CL-12345</t>
+  </si>
+  <si>
+    <t>Acme Corporation International</t>
+  </si>
+  <si>
+    <t>photo_a.jpg</t>
+  </si>
+  <si>
+    <t>signature.png</t>
+  </si>
+  <si>
+    <t>CL-98765</t>
+  </si>
+  <si>
+    <t>Jane Doe Enterprises LLC</t>
+  </si>
+  <si>
+    <t>photo_b.jpg</t>
+  </si>
+  <si>
+    <t>None</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+    <numFmt numFmtId="165" formatCode="$#,##0.00"/>
+  </numFmts>
+  <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -130,8 +115,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -426,110 +414,106 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" t="s">
+    <row r="1" spans="1:10">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" t="s">
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="2">
+        <v>45224</v>
+      </c>
+      <c r="D2" s="3">
+        <v>150000.5</v>
+      </c>
+      <c r="E2">
+        <v>0.985</v>
+      </c>
+      <c r="F2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>10</v>
+      </c>
+      <c r="I2" t="s">
         <v>12</v>
       </c>
-      <c r="E1" t="s">
+      <c r="J2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="2">
+        <v>45306</v>
+      </c>
+      <c r="D3" s="3">
+        <v>2500</v>
+      </c>
+      <c r="E3">
+        <v>0.45</v>
+      </c>
+      <c r="F3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>20</v>
+      </c>
+      <c r="I3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" t="s">
         <v>17</v>
-      </c>
-      <c r="F1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>15000.5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>2500</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>1000000</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New templates for exhaustive testing
</commit_message>
<xml_diff>
--- a/data/mock_data/mock_data.xlsx
+++ b/data/mock_data/mock_data.xlsx
@@ -14,60 +14,135 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
-  <si>
-    <t>client_id</t>
-  </si>
-  <si>
-    <t>client_name</t>
-  </si>
-  <si>
-    <t>contract_date</t>
-  </si>
-  <si>
-    <t>contract_value</t>
-  </si>
-  <si>
-    <t>completion_rate</t>
-  </si>
-  <si>
-    <t>is_active</t>
-  </si>
-  <si>
-    <t>has_debt</t>
-  </si>
-  <si>
-    <t>status_code</t>
-  </si>
-  <si>
-    <t>client_photo</t>
-  </si>
-  <si>
-    <t>signature_img</t>
-  </si>
-  <si>
-    <t>CL-12345</t>
-  </si>
-  <si>
-    <t>Acme Corporation International</t>
-  </si>
-  <si>
-    <t>photo_a.jpg</t>
-  </si>
-  <si>
-    <t>signature.png</t>
-  </si>
-  <si>
-    <t>CL-98765</t>
-  </si>
-  <si>
-    <t>Jane Doe Enterprises LLC</t>
-  </si>
-  <si>
-    <t>photo_b.jpg</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="43">
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>company</t>
+  </si>
+  <si>
+    <t>ceo_name</t>
+  </si>
+  <si>
+    <t>founded_date</t>
+  </si>
+  <si>
+    <t>revenue_q4</t>
+  </si>
+  <si>
+    <t>growth_pct</t>
+  </si>
+  <si>
+    <t>is_public</t>
+  </si>
+  <si>
+    <t>compliance_check</t>
+  </si>
+  <si>
+    <t>risk_score</t>
+  </si>
+  <si>
+    <t>email_contact</t>
+  </si>
+  <si>
+    <t>card_token</t>
+  </si>
+  <si>
+    <t>logo_img</t>
+  </si>
+  <si>
+    <t>ceo_img</t>
+  </si>
+  <si>
+    <t>auth_sig</t>
+  </si>
+  <si>
+    <t>CORP-001</t>
+  </si>
+  <si>
+    <t>Acme Solutions Inc.</t>
+  </si>
+  <si>
+    <t>John Sterling</t>
+  </si>
+  <si>
+    <t>contact@acme.com</t>
+  </si>
+  <si>
+    <t>4532123456789012</t>
+  </si>
+  <si>
+    <t>logo_acme.png</t>
+  </si>
+  <si>
+    <t>profile_CEO.jpg</t>
+  </si>
+  <si>
+    <t>sig_valid.png</t>
+  </si>
+  <si>
+    <t>CORP-002</t>
+  </si>
+  <si>
+    <t>Omega G.m.b.H</t>
+  </si>
+  <si>
+    <t>Klaus Müller</t>
+  </si>
+  <si>
+    <t>info@omega.de</t>
+  </si>
+  <si>
+    <t>5500123456789012</t>
   </si>
   <si>
     <t>None</t>
+  </si>
+  <si>
+    <t>profile_CTO.jpg</t>
+  </si>
+  <si>
+    <t>CORP-003</t>
+  </si>
+  <si>
+    <t>Cyberdyne Sys</t>
+  </si>
+  <si>
+    <t>Sarah Connor</t>
+  </si>
+  <si>
+    <t>alert@skynet.net</t>
+  </si>
+  <si>
+    <t>371234567890123</t>
+  </si>
+  <si>
+    <t>chart_growth.jpg</t>
+  </si>
+  <si>
+    <t>CORP-004</t>
+  </si>
+  <si>
+    <t>Stealth Startup</t>
+  </si>
+  <si>
+    <t>1234</t>
+  </si>
+  <si>
+    <t>CORP-005</t>
+  </si>
+  <si>
+    <t>The Very Long Company Name Limited Partnership Global Edition</t>
+  </si>
+  <si>
+    <t>Alexander Wolfeschlegelsteinhausenbergerdorff</t>
+  </si>
+  <si>
+    <t>ceo@verylongdomainnamecompany.com</t>
+  </si>
+  <si>
+    <t>4111111111111111</t>
   </si>
 </sst>
 </file>
@@ -89,21 +164,27 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF2C3E50"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -111,15 +192,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -414,13 +513,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="14" width="20.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -451,69 +553,233 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:10">
-      <c r="A2" t="s">
+    <row r="2" spans="1:14">
+      <c r="A2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="3">
+        <v>35927</v>
+      </c>
+      <c r="E2" s="4">
+        <v>1500000</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0.125</v>
+      </c>
+      <c r="G2" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H2" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I2" s="2">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="2">
-        <v>45224</v>
-      </c>
-      <c r="D2" s="3">
-        <v>150000.5</v>
-      </c>
-      <c r="E2">
-        <v>0.985</v>
-      </c>
-      <c r="F2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G2" t="b">
+      <c r="J2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="3">
+        <v>38686</v>
+      </c>
+      <c r="E3" s="4">
+        <v>450500.5</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0.052</v>
+      </c>
+      <c r="G3" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="H2">
+      <c r="H3" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I3" s="2">
+        <v>20</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="3">
+        <v>45292</v>
+      </c>
+      <c r="E4" s="4">
+        <v>-50000</v>
+      </c>
+      <c r="F4" s="4">
+        <v>-0.25</v>
+      </c>
+      <c r="G4" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H4" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I4" s="2">
+        <v>30</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="3">
+        <v>45658</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0</v>
+      </c>
+      <c r="F5" s="4">
+        <v>0</v>
+      </c>
+      <c r="G5" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H5" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I5" s="2">
+        <v>99</v>
+      </c>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1</v>
+      </c>
+      <c r="E6" s="4">
+        <v>9999999.99</v>
+      </c>
+      <c r="F6" s="4">
+        <v>1</v>
+      </c>
+      <c r="G6" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H6" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I6" s="2">
         <v>10</v>
       </c>
-      <c r="I2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="2">
-        <v>45306</v>
-      </c>
-      <c r="D3" s="3">
-        <v>2500</v>
-      </c>
-      <c r="E3">
-        <v>0.45</v>
-      </c>
-      <c r="F3" t="b">
-        <v>0</v>
-      </c>
-      <c r="G3" t="b">
-        <v>1</v>
-      </c>
-      <c r="H3">
+      <c r="J6" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="I3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J3" t="s">
-        <v>17</v>
+      <c r="N6" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>